<commit_message>
some ecomic analysis on utility streams
</commit_message>
<xml_diff>
--- a/Economics/Design_Specs.xlsx
+++ b/Economics/Design_Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wylie/Desktop/UW/CHEME485_ProcessDesign/Wi2020_CHEME485_FinalProject/Economics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29F4961-4C2B-0F4F-8114-268209B4AD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB80E02-92C6-AE43-9953-7F3646C469B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{CFA67F1E-3B02-45DC-B7E7-BEEA5ACEE9D7}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{CFA67F1E-3B02-45DC-B7E7-BEEA5ACEE9D7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>util</t>
   </si>
@@ -127,13 +127,58 @@
   </si>
   <si>
     <t>$/GJ</t>
+  </si>
+  <si>
+    <t>kJ/mol</t>
+  </si>
+  <si>
+    <t>g/mol</t>
+  </si>
+  <si>
+    <t>kJ/g</t>
+  </si>
+  <si>
+    <t>kJ/kg</t>
+  </si>
+  <si>
+    <t>kJ/tonne</t>
+  </si>
+  <si>
+    <t>O-xylene Enthalpy of combustion</t>
+  </si>
+  <si>
+    <t>If we assume that the boiler feed water we use to cool our very hot processes is simply used to vaporize the boiler feed water we feed it, we can get a cost/GJ cooling for using BFW</t>
+  </si>
+  <si>
+    <t>$/1000 kg</t>
+  </si>
+  <si>
+    <t>Enthalpy of vaporization</t>
+  </si>
+  <si>
+    <t>GJ/tonne</t>
+  </si>
+  <si>
+    <t>$/GJ cooling</t>
+  </si>
+  <si>
+    <t>In stream 16, we are losing 9.337 kmol/hr (as a purge). We can burn this to produce some of the steam required elsewhere</t>
+  </si>
+  <si>
+    <t>BFW available at 115 c - used for cooling in E-705 through 706</t>
+  </si>
+  <si>
+    <t>kmol/hr purged</t>
+  </si>
+  <si>
+    <t>kJ/hr energy we can use</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +196,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,9 +237,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,22 +558,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A48BFDD-CE5C-469D-A3F1-E46D52F0D175}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-4552</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>106.16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f>A6/A7</f>
+        <v>-42.87867370007536</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>A8*1000</f>
+        <v>-42878.673700075364</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f>A9*1000</f>
+        <v>-42878673.700075366</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9.3369999999999997</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f>A11*A6*1000</f>
+        <v>-42502024</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>40.65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f>A18/A19</f>
+        <v>2.2583333333333333</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f>A20*1000</f>
+        <v>2258.3333333333335</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f>A21*1000</f>
+        <v>2258333.3333333335</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f>A22/1000000</f>
+        <v>2.2583333333333333</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <f>A16/A23</f>
+        <v>1.0848708487084873</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -518,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DADDF4-B8B2-495E-92C3-A07FC1C62266}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="71" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -655,6 +878,9 @@
       <c r="G4" t="s">
         <v>12</v>
       </c>
+      <c r="H4">
+        <v>14.19</v>
+      </c>
       <c r="I4">
         <f>400</f>
         <v>400</v>
@@ -687,6 +913,9 @@
       <c r="G5" t="s">
         <v>15</v>
       </c>
+      <c r="H5">
+        <v>1.08</v>
+      </c>
       <c r="I5">
         <f>400</f>
         <v>400</v>
@@ -716,6 +945,9 @@
       <c r="G6" t="s">
         <v>15</v>
       </c>
+      <c r="H6">
+        <v>1.08</v>
+      </c>
       <c r="I6">
         <f>400</f>
         <v>400</v>
@@ -745,6 +977,9 @@
       <c r="G7" t="s">
         <v>15</v>
       </c>
+      <c r="H7">
+        <v>1.08</v>
+      </c>
       <c r="I7">
         <f>400</f>
         <v>400</v>
@@ -753,6 +988,9 @@
         <f t="shared" si="0"/>
         <v>13.811216350947156</v>
       </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -849,11 +1087,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F55A5E-412B-E445-BCB1-EFBA77B9B60E}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Updated calcs, CAPCOST for equip list (not utils)
</commit_message>
<xml_diff>
--- a/Economics/Design_Specs.xlsx
+++ b/Economics/Design_Specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wylie/Desktop/UW/CHEME485_ProcessDesign/Wi2020_CHEME485_FinalProject/Economics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kauib\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB80E02-92C6-AE43-9953-7F3646C469B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C4E1219-B32C-4B12-9DA4-82A055779AD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{CFA67F1E-3B02-45DC-B7E7-BEEA5ACEE9D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CFA67F1E-3B02-45DC-B7E7-BEEA5ACEE9D7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>util</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>kJ/hr energy we can use</t>
+  </si>
+  <si>
+    <t>Duty (MJ/h)</t>
   </si>
 </sst>
 </file>
@@ -561,36 +564,36 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>-4552</v>
       </c>
@@ -598,7 +601,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>106.16</v>
       </c>
@@ -606,7 +609,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <f>A6/A7</f>
         <v>-42.87867370007536</v>
@@ -615,7 +618,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <f>A8*1000</f>
         <v>-42878.673700075364</v>
@@ -624,7 +627,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <f>A9*1000</f>
         <v>-42878673.700075366</v>
@@ -633,7 +636,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9.3369999999999997</v>
       </c>
@@ -641,7 +644,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <f>A11*A6*1000</f>
         <v>-42502024</v>
@@ -650,17 +653,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2.4500000000000002</v>
       </c>
@@ -668,12 +671,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>40.65</v>
       </c>
@@ -681,7 +684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -689,7 +692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <f>A18/A19</f>
         <v>2.2583333333333333</v>
@@ -698,7 +701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <f>A20*1000</f>
         <v>2258.3333333333335</v>
@@ -707,7 +710,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <f>A21*1000</f>
         <v>2258333.3333333335</v>
@@ -716,7 +719,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <f>A22/1000000</f>
         <v>2.2583333333333333</v>
@@ -725,7 +728,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <f>A16/A23</f>
         <v>1.0848708487084873</v>
@@ -741,19 +744,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DADDF4-B8B2-495E-92C3-A07FC1C62266}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="71" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -761,31 +765,34 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -793,34 +800,38 @@
         <v>4447.8999999999996</v>
       </c>
       <c r="C2">
+        <f>B2*3.6</f>
+        <v>16012.439999999999</v>
+      </c>
+      <c r="D2">
         <v>134.19999999999999</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>154.69999999999999</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>184</v>
       </c>
-      <c r="F2">
-        <f>((E2-C2)-(E2-D2))/LN((E2-C2)/(E2-D2))</f>
+      <c r="G2">
+        <f>((F2-D2)-(F2-E2))/LN((F2-D2)/(F2-E2))</f>
         <v>38.64807393365767</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>14.19</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J7" si="0">B2*1000/(F2*I2)</f>
+      <c r="K2">
+        <f>B2*1000/(G2*J2)</f>
         <v>287.71808962816334</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -828,34 +839,38 @@
         <v>-18194.2</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:C7" si="0">B3*3.6</f>
+        <v>-65499.12</v>
+      </c>
+      <c r="D3">
         <v>400</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>110</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>35</v>
       </c>
-      <c r="F3">
-        <f>((E3-C3)-(E3-D3))/LN((E3-C3)/(E3-D3))</f>
+      <c r="G3">
+        <f>((F3-D3)-(F3-E3))/LN((F3-D3)/(F3-E3))</f>
         <v>-183.26485504567495</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.35399999999999998</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
+      <c r="K3">
+        <f>B3*1000/(G3*J3)</f>
         <v>248.1954327176571</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -863,34 +878,38 @@
         <v>2800.47</v>
       </c>
       <c r="C4">
+        <f t="shared" si="0"/>
+        <v>10081.691999999999</v>
+      </c>
+      <c r="D4">
         <v>110</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>180</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>184</v>
       </c>
-      <c r="F4">
-        <f>((E4-C4)-(E4-D4))/LN((E4-C4)/(E4-D4))</f>
+      <c r="G4">
+        <f>((F4-D4)-(F4-E4))/LN((F4-D4)/(F4-E4))</f>
         <v>23.990918556509143</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>14.19</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
+      <c r="K4">
+        <f>B4*1000/(G4*J4)</f>
         <v>291.82605007428793</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -898,98 +917,110 @@
         <v>-439.5</v>
       </c>
       <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-1582.2</v>
+      </c>
+      <c r="D5">
         <v>264</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>210</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>115</v>
       </c>
-      <c r="F5">
-        <f>((E5-C5)-(E5-D5))/LN((E5-C5)/(E5-D5))</f>
+      <c r="G5">
+        <f>((F5-D5)-(F5-E5))/LN((F5-D5)/(F5-E5))</f>
         <v>-119.98149236290068</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1.08</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
+      <c r="K5">
+        <f>B5*1000/(G5*J5)</f>
         <v>9.1576623891014624</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
         <v>-3355.5</v>
       </c>
-      <c r="D6">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-12079.800000000001</v>
+      </c>
+      <c r="E6">
         <v>159</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>115</v>
       </c>
-      <c r="F6">
-        <f>E6-D6</f>
+      <c r="G6">
+        <f>F6-E6</f>
         <v>-44</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1.08</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
+      <c r="K6">
+        <f>B6*1000/(G6*J6)</f>
         <v>190.65340909090909</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7">
         <v>-554.10599999999999</v>
       </c>
-      <c r="D7">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-1994.7816</v>
+      </c>
+      <c r="E7">
         <v>215.3</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>115</v>
       </c>
-      <c r="F7">
-        <f>E7-D7</f>
+      <c r="G7">
+        <f>F7-E7</f>
         <v>-100.30000000000001</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>15</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1.08</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
+      <c r="K7">
+        <f>B7*1000/(G7*J7)</f>
         <v>13.811216350947156</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" s="2"/>
     </row>
   </sheetData>
@@ -1003,15 +1034,15 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1028,12 +1059,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>0.55000000000000004</v>
@@ -1043,10 +1074,10 @@
       </c>
       <c r="E2">
         <f>B2*C2+3</f>
-        <v>21.150000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1077,7 +1108,7 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1091,13 +1122,13 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>